<commit_message>
BRANLE BURNES DOIT CHANGER TAILLE IMAGES
</commit_message>
<xml_diff>
--- a/src/main/resources/gmr_templ_2016.xlsx
+++ b/src/main/resources/gmr_templ_2016.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7230"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
     <sheet name="GRP" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -332,11 +332,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _H_U_F_-;\-* #,##0.00\ _H_U_F_-;_-* &quot;-&quot;??\ _H_U_F_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0\ _H_U_F_-;\-* #,##0\ _H_U_F_-;_-* &quot;-&quot;??\ _H_U_F_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _H_U_F_-;\-* #,##0.00\ _H_U_F_-;_-* &quot;-&quot;??\ _H_U_F_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0\ _H_U_F_-;\-* #,##0\ _H_U_F_-;_-* &quot;-&quot;??\ _H_U_F_-;_-@_-"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -1112,7 +1112,7 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -1302,13 +1302,31 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="33" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="32" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1349,31 +1367,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="33" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="32" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Ezres" xfId="2" builtinId="3"/>
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normál 2" xfId="1"/>
     <cellStyle name="Normál 3" xfId="3"/>
-    <cellStyle name="Százalék" xfId="4" builtinId="5"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1389,7 +1389,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1464,23 +1464,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1516,23 +1499,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1711,8 +1677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I84" sqref="I84"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,9 +1781,9 @@
       </c>
       <c r="B14" s="60"/>
       <c r="C14" s="62"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="103"/>
-      <c r="F14" s="104"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="110"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="63">
@@ -1827,9 +1793,9 @@
         <v>56</v>
       </c>
       <c r="C15" s="64"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="107"/>
+      <c r="D15" s="111"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="113"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1934,16 +1900,16 @@
       <c r="A27" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="113">
+      <c r="B27" s="102">
         <v>1.2</v>
       </c>
-      <c r="C27" s="113">
+      <c r="C27" s="102">
         <v>1.4</v>
       </c>
-      <c r="D27" s="113">
+      <c r="D27" s="102">
         <v>1</v>
       </c>
-      <c r="E27" s="113">
+      <c r="E27" s="102">
         <v>0.1</v>
       </c>
     </row>
@@ -1951,16 +1917,16 @@
       <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="114">
+      <c r="B28" s="103">
         <v>0.87</v>
       </c>
-      <c r="C28" s="114">
+      <c r="C28" s="103">
         <v>0.76</v>
       </c>
-      <c r="D28" s="114">
+      <c r="D28" s="103">
         <v>0.3</v>
       </c>
-      <c r="E28" s="114">
+      <c r="E28" s="103">
         <v>0.87</v>
       </c>
     </row>
@@ -2041,38 +2007,38 @@
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="35"/>
+      <c r="B36" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="37" spans="1:5" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="69" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="70" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="113">
+      <c r="B38" s="102">
         <v>1.2</v>
       </c>
-      <c r="C38" s="113">
+      <c r="C38" s="102">
         <v>1.4</v>
       </c>
-      <c r="D38" s="113">
+      <c r="D38" s="102">
         <v>1</v>
       </c>
-      <c r="E38" s="113">
+      <c r="E38" s="102">
         <v>0.1</v>
       </c>
     </row>
@@ -2080,16 +2046,16 @@
       <c r="A39" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="114">
+      <c r="B39" s="103">
         <v>0.87</v>
       </c>
-      <c r="C39" s="114">
+      <c r="C39" s="103">
         <v>0.76</v>
       </c>
-      <c r="D39" s="114">
+      <c r="D39" s="103">
         <v>0.3</v>
       </c>
-      <c r="E39" s="114">
+      <c r="E39" s="103">
         <v>0.87</v>
       </c>
     </row>
@@ -2269,16 +2235,16 @@
       <c r="A55" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="115">
+      <c r="B55" s="104">
         <v>0.2</v>
       </c>
-      <c r="C55" s="115">
+      <c r="C55" s="104">
         <v>0.2</v>
       </c>
-      <c r="D55" s="115">
+      <c r="D55" s="104">
         <v>0.2</v>
       </c>
-      <c r="E55" s="115">
+      <c r="E55" s="104">
         <v>0.2</v>
       </c>
     </row>
@@ -2286,16 +2252,16 @@
       <c r="A56" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="116">
+      <c r="B56" s="105">
         <v>1.2</v>
       </c>
-      <c r="C56" s="115">
+      <c r="C56" s="104">
         <v>1.2</v>
       </c>
-      <c r="D56" s="115">
+      <c r="D56" s="104">
         <v>1.2</v>
       </c>
-      <c r="E56" s="115">
+      <c r="E56" s="104">
         <v>1.2</v>
       </c>
     </row>
@@ -2303,16 +2269,16 @@
       <c r="A57" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B57" s="116">
+      <c r="B57" s="105">
         <v>0.76</v>
       </c>
-      <c r="C57" s="115">
+      <c r="C57" s="104">
         <v>0.76</v>
       </c>
-      <c r="D57" s="115">
+      <c r="D57" s="104">
         <v>0.76</v>
       </c>
-      <c r="E57" s="115">
+      <c r="E57" s="104">
         <v>0.76</v>
       </c>
     </row>
@@ -2320,16 +2286,16 @@
       <c r="A58" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B58" s="116">
+      <c r="B58" s="105">
         <v>0.98</v>
       </c>
-      <c r="C58" s="115">
+      <c r="C58" s="104">
         <v>0.98</v>
       </c>
-      <c r="D58" s="115">
+      <c r="D58" s="104">
         <v>0.98</v>
       </c>
-      <c r="E58" s="115">
+      <c r="E58" s="104">
         <v>0.98</v>
       </c>
     </row>
@@ -2337,16 +2303,16 @@
       <c r="A59" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="116">
+      <c r="B59" s="105">
         <v>1</v>
       </c>
-      <c r="C59" s="115">
+      <c r="C59" s="104">
         <v>1</v>
       </c>
-      <c r="D59" s="115">
+      <c r="D59" s="104">
         <v>1</v>
       </c>
-      <c r="E59" s="115">
+      <c r="E59" s="104">
         <v>1</v>
       </c>
     </row>
@@ -2354,16 +2320,16 @@
       <c r="A60" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B60" s="117">
+      <c r="B60" s="106">
         <v>0.88</v>
       </c>
-      <c r="C60" s="115">
+      <c r="C60" s="104">
         <v>0.88</v>
       </c>
-      <c r="D60" s="115">
+      <c r="D60" s="104">
         <v>0.88</v>
       </c>
-      <c r="E60" s="115">
+      <c r="E60" s="104">
         <v>0.88</v>
       </c>
     </row>
@@ -2534,16 +2500,16 @@
       <c r="A74" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B74" s="115">
+      <c r="B74" s="104">
         <v>0.2</v>
       </c>
-      <c r="C74" s="113">
+      <c r="C74" s="102">
         <v>0.2</v>
       </c>
-      <c r="D74" s="113">
+      <c r="D74" s="102">
         <v>0.2</v>
       </c>
-      <c r="E74" s="115">
+      <c r="E74" s="104">
         <v>0.2</v>
       </c>
     </row>
@@ -2551,16 +2517,16 @@
       <c r="A75" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B75" s="116">
+      <c r="B75" s="105">
         <v>1.2</v>
       </c>
-      <c r="C75" s="118">
+      <c r="C75" s="107">
         <v>1.2</v>
       </c>
-      <c r="D75" s="118">
+      <c r="D75" s="107">
         <v>1.2</v>
       </c>
-      <c r="E75" s="116">
+      <c r="E75" s="105">
         <v>1.2</v>
       </c>
     </row>
@@ -2568,16 +2534,16 @@
       <c r="A76" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B76" s="116">
+      <c r="B76" s="105">
         <v>0.76</v>
       </c>
-      <c r="C76" s="118">
+      <c r="C76" s="107">
         <v>0.76</v>
       </c>
-      <c r="D76" s="118">
+      <c r="D76" s="107">
         <v>0.76</v>
       </c>
-      <c r="E76" s="116">
+      <c r="E76" s="105">
         <v>0.76</v>
       </c>
     </row>
@@ -2585,16 +2551,16 @@
       <c r="A77" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B77" s="116">
+      <c r="B77" s="105">
         <v>0.98</v>
       </c>
-      <c r="C77" s="118">
+      <c r="C77" s="107">
         <v>0.98</v>
       </c>
-      <c r="D77" s="118">
+      <c r="D77" s="107">
         <v>0.98</v>
       </c>
-      <c r="E77" s="116">
+      <c r="E77" s="105">
         <v>0.98</v>
       </c>
     </row>
@@ -2602,16 +2568,16 @@
       <c r="A78" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B78" s="117">
+      <c r="B78" s="106">
         <v>1</v>
       </c>
-      <c r="C78" s="114">
+      <c r="C78" s="103">
         <v>1</v>
       </c>
-      <c r="D78" s="114">
+      <c r="D78" s="103">
         <v>1</v>
       </c>
-      <c r="E78" s="117">
+      <c r="E78" s="106">
         <v>1</v>
       </c>
     </row>
@@ -2765,16 +2731,16 @@
       <c r="A93" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B93" s="116">
+      <c r="B93" s="105">
         <v>0.2</v>
       </c>
-      <c r="C93" s="116">
+      <c r="C93" s="105">
         <v>0.2</v>
       </c>
-      <c r="D93" s="116">
+      <c r="D93" s="105">
         <v>0.2</v>
       </c>
-      <c r="E93" s="115">
+      <c r="E93" s="104">
         <v>0.2</v>
       </c>
     </row>
@@ -2782,16 +2748,16 @@
       <c r="A94" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B94" s="116">
+      <c r="B94" s="105">
         <v>1.2</v>
       </c>
-      <c r="C94" s="116">
+      <c r="C94" s="105">
         <v>1.2</v>
       </c>
-      <c r="D94" s="116">
+      <c r="D94" s="105">
         <v>1.2</v>
       </c>
-      <c r="E94" s="116">
+      <c r="E94" s="105">
         <v>1.2</v>
       </c>
     </row>
@@ -2799,16 +2765,16 @@
       <c r="A95" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B95" s="116">
+      <c r="B95" s="105">
         <v>0.76</v>
       </c>
-      <c r="C95" s="116">
+      <c r="C95" s="105">
         <v>0.76</v>
       </c>
-      <c r="D95" s="116">
+      <c r="D95" s="105">
         <v>0.76</v>
       </c>
-      <c r="E95" s="116">
+      <c r="E95" s="105">
         <v>0.76</v>
       </c>
     </row>
@@ -2816,16 +2782,16 @@
       <c r="A96" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B96" s="116">
+      <c r="B96" s="105">
         <v>0.98</v>
       </c>
-      <c r="C96" s="116">
+      <c r="C96" s="105">
         <v>0.98</v>
       </c>
-      <c r="D96" s="116">
+      <c r="D96" s="105">
         <v>0.98</v>
       </c>
-      <c r="E96" s="116">
+      <c r="E96" s="105">
         <v>0.98</v>
       </c>
     </row>
@@ -2945,7 +2911,7 @@
         <v>0.15260000000000001</v>
       </c>
       <c r="E106" s="9">
-        <v>0.22500000000000001</v>
+        <v>0.245</v>
       </c>
       <c r="F106" s="9">
         <v>7.3499999999999996E-2</v>
@@ -4571,408 +4537,408 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="114" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108" t="s">
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="108"/>
+      <c r="L1" s="114"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108" t="s">
+      <c r="B3" s="114"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108"/>
+      <c r="H3" s="114"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="114"/>
+      <c r="K3" s="114"/>
+      <c r="L3" s="114"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="115" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="108"/>
-      <c r="K5" s="108"/>
-      <c r="L5" s="108"/>
+      <c r="B5" s="114"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
+      <c r="I5" s="114"/>
+      <c r="J5" s="114"/>
+      <c r="K5" s="114"/>
+      <c r="L5" s="114"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="115" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="108"/>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="109" t="s">
+      <c r="B6" s="114"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="115" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="108"/>
-      <c r="L6" s="108"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="114"/>
+      <c r="K6" s="114"/>
+      <c r="L6" s="114"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="108" t="s">
+      <c r="A7" s="114" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="108"/>
-      <c r="C7" s="108"/>
-      <c r="D7" s="108"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="108">
+      <c r="B7" s="114"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="114"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="114">
         <v>5.2016</v>
       </c>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
-      <c r="J7" s="108"/>
-      <c r="K7" s="108"/>
-      <c r="L7" s="108"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="114"/>
+      <c r="K7" s="114"/>
+      <c r="L7" s="114"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="115" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="108"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108"/>
-      <c r="F9" s="108"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="108"/>
-      <c r="I9" s="108"/>
-      <c r="J9" s="108"/>
-      <c r="K9" s="108"/>
-      <c r="L9" s="108"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="114"/>
+      <c r="L9" s="114"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="109" t="s">
+      <c r="A10" s="115" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="108"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108"/>
-      <c r="F10" s="108"/>
-      <c r="G10" s="109" t="s">
+      <c r="B10" s="114"/>
+      <c r="C10" s="114"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="115" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="108"/>
-      <c r="I10" s="108"/>
-      <c r="J10" s="108"/>
-      <c r="K10" s="108"/>
-      <c r="L10" s="108"/>
+      <c r="H10" s="114"/>
+      <c r="I10" s="114"/>
+      <c r="J10" s="114"/>
+      <c r="K10" s="114"/>
+      <c r="L10" s="114"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="108" t="s">
+      <c r="A11" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="108"/>
-      <c r="C11" s="108"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="108"/>
-      <c r="F11" s="108"/>
-      <c r="G11" s="108" t="s">
+      <c r="B11" s="114"/>
+      <c r="C11" s="114"/>
+      <c r="D11" s="114"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="114"/>
+      <c r="G11" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="H11" s="108"/>
-      <c r="I11" s="108"/>
-      <c r="J11" s="108"/>
-      <c r="K11" s="108"/>
-      <c r="L11" s="108"/>
+      <c r="H11" s="114"/>
+      <c r="I11" s="114"/>
+      <c r="J11" s="114"/>
+      <c r="K11" s="114"/>
+      <c r="L11" s="114"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="109" t="s">
+      <c r="A13" s="115" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="108"/>
-      <c r="C13" s="108"/>
-      <c r="D13" s="108"/>
-      <c r="E13" s="108"/>
-      <c r="F13" s="108"/>
-      <c r="G13" s="108"/>
-      <c r="H13" s="108"/>
-      <c r="I13" s="108"/>
-      <c r="J13" s="108"/>
-      <c r="K13" s="108"/>
-      <c r="L13" s="108"/>
+      <c r="B13" s="114"/>
+      <c r="C13" s="114"/>
+      <c r="D13" s="114"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="114"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="114"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="114"/>
+      <c r="K13" s="114"/>
+      <c r="L13" s="114"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="109" t="s">
+      <c r="A14" s="115" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="108"/>
-      <c r="C14" s="108"/>
-      <c r="D14" s="109" t="s">
+      <c r="B14" s="114"/>
+      <c r="C14" s="114"/>
+      <c r="D14" s="115" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="108"/>
-      <c r="F14" s="108"/>
-      <c r="G14" s="109" t="s">
+      <c r="E14" s="114"/>
+      <c r="F14" s="114"/>
+      <c r="G14" s="115" t="s">
         <v>82</v>
       </c>
-      <c r="H14" s="108"/>
-      <c r="I14" s="109" t="s">
+      <c r="H14" s="114"/>
+      <c r="I14" s="115" t="s">
         <v>83</v>
       </c>
-      <c r="J14" s="108"/>
-      <c r="K14" s="109" t="s">
+      <c r="J14" s="114"/>
+      <c r="K14" s="115" t="s">
         <v>84</v>
       </c>
-      <c r="L14" s="108"/>
+      <c r="L14" s="114"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="108" t="s">
+      <c r="A15" s="114" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="108"/>
-      <c r="C15" s="108"/>
-      <c r="D15" s="108" t="s">
+      <c r="B15" s="114"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="108"/>
-      <c r="F15" s="108"/>
-      <c r="G15" s="108" t="s">
+      <c r="E15" s="114"/>
+      <c r="F15" s="114"/>
+      <c r="G15" s="114" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="108"/>
-      <c r="I15" s="108" t="s">
+      <c r="H15" s="114"/>
+      <c r="I15" s="114" t="s">
         <v>85</v>
       </c>
-      <c r="J15" s="108"/>
-      <c r="K15" s="108">
+      <c r="J15" s="114"/>
+      <c r="K15" s="114">
         <v>3712538</v>
       </c>
-      <c r="L15" s="108"/>
+      <c r="L15" s="114"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="108" t="s">
+      <c r="A16" s="114" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="108"/>
-      <c r="C16" s="108"/>
-      <c r="D16" s="108" t="s">
+      <c r="B16" s="114"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="108"/>
-      <c r="F16" s="108"/>
-      <c r="G16" s="108" t="s">
+      <c r="E16" s="114"/>
+      <c r="F16" s="114"/>
+      <c r="G16" s="114" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="108"/>
-      <c r="I16" s="108" t="s">
+      <c r="H16" s="114"/>
+      <c r="I16" s="114" t="s">
         <v>86</v>
       </c>
-      <c r="J16" s="108"/>
-      <c r="K16" s="108">
+      <c r="J16" s="114"/>
+      <c r="K16" s="114">
         <v>3351129</v>
       </c>
-      <c r="L16" s="108"/>
+      <c r="L16" s="114"/>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A17" s="108" t="s">
+      <c r="A17" s="114" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="108"/>
-      <c r="C17" s="108"/>
-      <c r="D17" s="108" t="s">
+      <c r="B17" s="114"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="108"/>
-      <c r="F17" s="108"/>
-      <c r="G17" s="108" t="s">
+      <c r="E17" s="114"/>
+      <c r="F17" s="114"/>
+      <c r="G17" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="108"/>
-      <c r="I17" s="108" t="s">
+      <c r="H17" s="114"/>
+      <c r="I17" s="114" t="s">
         <v>87</v>
       </c>
-      <c r="J17" s="108"/>
-      <c r="K17" s="108">
+      <c r="J17" s="114"/>
+      <c r="K17" s="114">
         <v>2645503</v>
       </c>
-      <c r="L17" s="108"/>
+      <c r="L17" s="114"/>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A18" s="108" t="s">
+      <c r="A18" s="114" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="108"/>
-      <c r="C18" s="108"/>
-      <c r="D18" s="108" t="s">
+      <c r="B18" s="114"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="108"/>
-      <c r="F18" s="108"/>
-      <c r="G18" s="108" t="s">
+      <c r="E18" s="114"/>
+      <c r="F18" s="114"/>
+      <c r="G18" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="108"/>
-      <c r="I18" s="108" t="s">
+      <c r="H18" s="114"/>
+      <c r="I18" s="114" t="s">
         <v>88</v>
       </c>
-      <c r="J18" s="108"/>
-      <c r="K18" s="108">
+      <c r="J18" s="114"/>
+      <c r="K18" s="114">
         <v>352832</v>
       </c>
-      <c r="L18" s="108"/>
+      <c r="L18" s="114"/>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A20" s="110" t="s">
+      <c r="A20" s="116" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="110"/>
-      <c r="C20" s="110"/>
-      <c r="D20" s="110"/>
-      <c r="E20" s="110"/>
-      <c r="F20" s="110"/>
-      <c r="G20" s="110"/>
-      <c r="H20" s="110"/>
-      <c r="I20" s="110"/>
-      <c r="J20" s="110"/>
-      <c r="K20" s="110"/>
-      <c r="L20" s="110"/>
-      <c r="M20" s="110"/>
-      <c r="N20" s="110"/>
-      <c r="O20" s="110"/>
-      <c r="P20" s="110"/>
-      <c r="Q20" s="110"/>
-      <c r="R20" s="110"/>
-      <c r="S20" s="110"/>
-      <c r="T20" s="110"/>
-      <c r="U20" s="110"/>
-      <c r="V20" s="110"/>
-      <c r="W20" s="110"/>
-      <c r="X20" s="110"/>
-      <c r="Y20" s="110"/>
-      <c r="Z20" s="110"/>
+      <c r="B20" s="116"/>
+      <c r="C20" s="116"/>
+      <c r="D20" s="116"/>
+      <c r="E20" s="116"/>
+      <c r="F20" s="116"/>
+      <c r="G20" s="116"/>
+      <c r="H20" s="116"/>
+      <c r="I20" s="116"/>
+      <c r="J20" s="116"/>
+      <c r="K20" s="116"/>
+      <c r="L20" s="116"/>
+      <c r="M20" s="116"/>
+      <c r="N20" s="116"/>
+      <c r="O20" s="116"/>
+      <c r="P20" s="116"/>
+      <c r="Q20" s="116"/>
+      <c r="R20" s="116"/>
+      <c r="S20" s="116"/>
+      <c r="T20" s="116"/>
+      <c r="U20" s="116"/>
+      <c r="V20" s="116"/>
+      <c r="W20" s="116"/>
+      <c r="X20" s="116"/>
+      <c r="Y20" s="116"/>
+      <c r="Z20" s="116"/>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A21" s="110" t="s">
+      <c r="A21" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="110" t="s">
+      <c r="B21" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="110" t="s">
+      <c r="C21" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="110" t="s">
+      <c r="D21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="110" t="s">
+      <c r="E21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="110" t="s">
+      <c r="F21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="110" t="s">
+      <c r="G21" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="H21" s="110" t="s">
+      <c r="H21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="I21" s="110" t="s">
+      <c r="I21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="J21" s="110" t="s">
+      <c r="J21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="K21" s="110" t="s">
+      <c r="K21" s="116" t="s">
         <v>67</v>
       </c>
-      <c r="L21" s="110" t="s">
+      <c r="L21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="M21" s="110" t="s">
+      <c r="M21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="N21" s="110" t="s">
+      <c r="N21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="O21" s="110" t="s">
+      <c r="O21" s="116" t="s">
         <v>68</v>
       </c>
-      <c r="P21" s="110" t="s">
+      <c r="P21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="Q21" s="110" t="s">
+      <c r="Q21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="R21" s="110" t="s">
+      <c r="R21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="S21" s="110" t="s">
+      <c r="S21" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="T21" s="110" t="s">
+      <c r="T21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="U21" s="110" t="s">
+      <c r="U21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="V21" s="110" t="s">
+      <c r="V21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="W21" s="110" t="s">
+      <c r="W21" s="116" t="s">
         <v>70</v>
       </c>
-      <c r="X21" s="110" t="s">
+      <c r="X21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="Y21" s="110" t="s">
+      <c r="Y21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="Z21" s="110" t="s">
+      <c r="Z21" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="AA21" s="111" t="s">
+      <c r="AA21" s="117" t="s">
         <v>71</v>
       </c>
-      <c r="AB21" s="111"/>
-      <c r="AC21" s="111"/>
-      <c r="AD21" s="111"/>
-      <c r="AE21" s="112" t="s">
+      <c r="AB21" s="117"/>
+      <c r="AC21" s="117"/>
+      <c r="AD21" s="117"/>
+      <c r="AE21" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="AF21" s="112"/>
-      <c r="AG21" s="112"/>
-      <c r="AH21" s="112"/>
+      <c r="AF21" s="118"/>
+      <c r="AG21" s="118"/>
+      <c r="AH21" s="118"/>
     </row>
     <row r="22" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="110" t="s">
+      <c r="A22" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="110" t="s">
+      <c r="B22" s="116" t="s">
         <v>63</v>
       </c>
       <c r="C22" s="82" t="s">
@@ -5073,7 +5039,7 @@
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A23" s="110" t="s">
+      <c r="A23" s="116" t="s">
         <v>75</v>
       </c>
       <c r="B23" s="83" t="s">
@@ -5177,7 +5143,7 @@
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A24" s="110" t="s">
+      <c r="A24" s="116" t="s">
         <v>65</v>
       </c>
       <c r="B24" s="83" t="s">
@@ -5281,7 +5247,7 @@
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A25" s="110" t="s">
+      <c r="A25" s="116" t="s">
         <v>65</v>
       </c>
       <c r="B25" s="82" t="s">
@@ -5385,22 +5351,22 @@
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A27" s="108" t="s">
+      <c r="A27" s="114" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="108"/>
-      <c r="C27" s="108"/>
-      <c r="D27" s="108"/>
-      <c r="E27" s="108"/>
-      <c r="F27" s="108"/>
-      <c r="G27" s="108"/>
-      <c r="H27" s="108"/>
-      <c r="I27" s="108"/>
-      <c r="J27" s="108"/>
-      <c r="K27" s="108" t="s">
+      <c r="B27" s="114"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="114"/>
+      <c r="E27" s="114"/>
+      <c r="F27" s="114"/>
+      <c r="G27" s="114"/>
+      <c r="H27" s="114"/>
+      <c r="I27" s="114"/>
+      <c r="J27" s="114"/>
+      <c r="K27" s="114" t="s">
         <v>61</v>
       </c>
-      <c r="L27" s="108"/>
+      <c r="L27" s="114"/>
       <c r="R27" s="95" t="s">
         <v>95</v>
       </c>

</xml_diff>